<commit_message>
added orderby employee_id in getlist
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -2,17 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="部署" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="役職" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3" state="visible"/>
+    <sheet name="部署" sheetId="2" r:id="rId4" state="visible"/>
+    <sheet name="役職" sheetId="3" r:id="rId5" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -41,24 +41,24 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <b/>
+        <color rgb="FF000000"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b/>
+        <color rgb="FF000000"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">電話番号</t>
     </r>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
@@ -182,7 +182,7 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
+      <b val="1"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC"/>
@@ -190,7 +190,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b val="1"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -226,7 +226,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b val="1"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Noto Sans CJK SC"/>
@@ -282,14 +282,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -299,8 +299,8 @@
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
@@ -324,64 +324,64 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="right" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="right" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -498,14 +498,14 @@
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial" pitchFamily="0"/>
+        <a:ea typeface="Arial" pitchFamily="0"/>
+        <a:cs typeface="Arial" pitchFamily="0"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial" pitchFamily="0"/>
+        <a:ea typeface="Arial" pitchFamily="0"/>
+        <a:cs typeface="Arial" pitchFamily="0"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -624,6 +624,8 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -8505,182 +8507,176 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C202 A1"/>
+    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C3:C202 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" ht="15.75">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" ht="15.75">
       <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" ht="15.75">
       <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="13"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" ht="15.75" customHeight="true">
       <c r="A5" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" ht="15.75" customHeight="true">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" ht="15.75" customHeight="true">
       <c r="A7" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" ht="15.75" customHeight="true">
       <c r="A8" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" ht="15.75" customHeight="true">
       <c r="A9" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" ht="15.75" customHeight="true">
       <c r="A10" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" ht="15.75" customHeight="true">
       <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" ht="15.75" customHeight="true">
       <c r="A12" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" ht="15.75" customHeight="true">
       <c r="A13" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" ht="15.75" customHeight="true">
       <c r="A14" s="14" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions gridLinesSet="true"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup cellComments="none" copies="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C202 A1"/>
+    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C3:C202 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" ht="15.75">
       <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" ht="15.75">
+      <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" ht="15.75">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="13"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" ht="15.75" customHeight="true">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" ht="15.75" customHeight="true">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" ht="15.75" customHeight="true">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" ht="15.75" customHeight="true">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" ht="15.75" customHeight="true">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" ht="15.75" customHeight="true">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" ht="15.75" customHeight="true">
+      <c r="A11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" ht="15.75" customHeight="true">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions gridLinesSet="true"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup cellComments="none" copies="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added employee_id by adding admin
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -22,7 +22,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+  <si>
+    <t xml:space="preserve">EmployeeID</t>
+  </si>
   <si>
     <t xml:space="preserve">名</t>
   </si>
@@ -73,6 +76,9 @@
     <t xml:space="preserve">メールアドレス</t>
   </si>
   <si>
+    <t xml:space="preserve">DK1003</t>
+  </si>
+  <si>
     <t xml:space="preserve">Suhrob1</t>
   </si>
   <si>
@@ -85,45 +91,27 @@
     <t xml:space="preserve">EMPLOYEE</t>
   </si>
   <si>
+    <t xml:space="preserve">経営管理部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketolog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK1004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob2</t>
+  </si>
+  <si>
     <t xml:space="preserve">人事部</t>
   </si>
   <si>
     <t xml:space="preserve">CEO</t>
   </si>
   <si>
-    <t xml:space="preserve">nima@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">経営管理部</t>
-  </si>
-  <si>
     <t xml:space="preserve">経理部</t>
   </si>
   <si>
@@ -167,9 +155,6 @@
   </si>
   <si>
     <t xml:space="preserve">Software Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marketolog</t>
   </si>
   <si>
     <t xml:space="preserve">Digital analiser</t>
@@ -665,336 +650,202 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:J11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I2" s="9" t="n">
         <v>1234567</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="B3" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I3" s="9" t="n">
         <v>1234567</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="9" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="9" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="9" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="9" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="9" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="9" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="9" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="9" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1032,74 +883,74 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1128,64 +979,64 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed crate by excell api
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,21 +22,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">EmployeeID</t>
   </si>
   <si>
+    <t xml:space="preserve">姓</t>
+  </si>
+  <si>
     <t xml:space="preserve">名</t>
   </si>
   <si>
-    <t xml:space="preserve">姓</t>
-  </si>
-  <si>
     <t xml:space="preserve">表示名</t>
   </si>
   <si>
-    <t xml:space="preserve">Role</t>
+    <t xml:space="preserve">権限 </t>
   </si>
   <si>
     <t xml:space="preserve">パスワード</t>
@@ -79,94 +79,25 @@
     <t xml:space="preserve">DK1003</t>
   </si>
   <si>
-    <t xml:space="preserve">Suhrob1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ahmedov</t>
   </si>
   <si>
+    <t xml:space="preserve">Suxrob1</t>
+  </si>
+  <si>
     <t xml:space="preserve">sakura</t>
   </si>
   <si>
     <t xml:space="preserve">EMPLOYEE</t>
   </si>
   <si>
-    <t xml:space="preserve">経営管理部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marketolog</t>
+    <t xml:space="preserve">広報部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEO</t>
   </si>
   <si>
     <t xml:space="preserve">nima@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK1004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suhrob2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">人事部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">経理部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">営業部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">広報部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">開発部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">マーケティング部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">営業二部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">事業部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">新規事業部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">部署A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">経理第二部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">総務部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progect Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital analiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marketing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director</t>
   </si>
 </sst>
 </file>
@@ -176,13 +107,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
+      <name val="Noto Sans CJK JP"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -211,7 +141,28 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK JP"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -252,13 +203,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Poppins"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC"/>
@@ -268,12 +212,11 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
+      <name val="Noto Sans CJK JP"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,12 +233,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF45818E"/>
         <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -340,7 +277,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,47 +294,55 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -652,200 +597,181 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="1" sqref="C:C H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="12.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="32.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="9" t="n">
+      <c r="I2" s="12" t="n">
         <v>1234567</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="9" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="6"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="6"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="6"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="6"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="6"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="6"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="6"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="6"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -873,85 +799,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.53"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>20</v>
-      </c>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="12"/>
+      <c r="A3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="12"/>
+      <c r="A4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="A5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
-        <v>24</v>
-      </c>
+      <c r="A6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>26</v>
-      </c>
+      <c r="A8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="A9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="A10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="A11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="A13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="A14" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -969,75 +870,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.53"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="12"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added filter oby by excell create func  except email unique
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
   <si>
     <t xml:space="preserve">EmployeeID</t>
   </si>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">メールアドレス</t>
   </si>
   <si>
-    <t xml:space="preserve">DK1003</t>
+    <t xml:space="preserve">DK01221</t>
   </si>
   <si>
     <t xml:space="preserve">Ahmedov</t>
@@ -91,13 +91,94 @@
     <t xml:space="preserve">EMPLOYEE</t>
   </si>
   <si>
-    <t xml:space="preserve">広報部</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nima@gmail.com</t>
+    <t xml:space="preserve">1-department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111111111uyf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima11@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK01222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111111112jhcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima12@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK01223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima13@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK01224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima14@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima15@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK01226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima16@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK01227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima17gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK01240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima18@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">７７７ｈ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nima19@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hghjs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">656789787hhg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">656789787h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">656789787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">098765432123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-stage</t>
   </si>
 </sst>
 </file>
@@ -113,6 +194,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK JP"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -141,15 +223,9 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Noto Sans CJK JP"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -188,6 +264,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK JP"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,6 +296,7 @@
       <color theme="1"/>
       <name val="Noto Sans CJK JP"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -277,7 +360,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -294,40 +377,36 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -595,191 +674,1347 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="1" sqref="C:C H22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="1" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="12" t="n">
-        <v>1234567</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>17</v>
       </c>
+      <c r="J2" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="9"/>
+      <c r="A3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="9"/>
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="10" t="n">
+        <v>11111111113</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="9"/>
+      <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="9"/>
+      <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="10" t="n">
+        <v>11111111115</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="9"/>
+      <c r="A7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="10" t="n">
+        <v>11111111116</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="9"/>
+      <c r="A8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="10" t="n">
+        <v>11111111117</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="10" t="n">
+        <v>11111111118</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="10" t="n">
+        <v>11111111119</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="9"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="6"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="7"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="7"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="7"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="7"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="7"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="7"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="7"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="7"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="6"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="7"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="6"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="7"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="6"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="7"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="6"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="7"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="6"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="7"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="6"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="7"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="6"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="7"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="6"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="7"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="6"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="7"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="7"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="6"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="7"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="6"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="7"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="6"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="6"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="7"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="6"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="6"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="7"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="6"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="7"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="6"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="10"/>
+      <c r="J76" s="7"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="6"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="7"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="6"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="7"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="6"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="10"/>
+      <c r="J79" s="7"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="6"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="10"/>
+      <c r="J80" s="7"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="6"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="7"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="6"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="10"/>
+      <c r="J82" s="7"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="6"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="7"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="6"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="7"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="6"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="10"/>
+      <c r="J85" s="7"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="6"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="10"/>
+      <c r="J86" s="7"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="6"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="10"/>
+      <c r="J87" s="7"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="6"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="10"/>
+      <c r="J88" s="7"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="6"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="7"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="6"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="7"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="6"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="7"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="6"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="10"/>
+      <c r="J92" s="7"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="6"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="7"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="6"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="9"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="7"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="6"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="7"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="6"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="10"/>
+      <c r="J96" s="7"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="6"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="9"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="7"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="6"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="10"/>
+      <c r="J98" s="7"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="6"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="10"/>
+      <c r="J99" s="7"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="6"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="9"/>
+      <c r="I100" s="10"/>
+      <c r="J100" s="7"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="6"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="9"/>
+      <c r="I101" s="10"/>
+      <c r="J101" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G11" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G101" type="list">
       <formula1>部署!$A$2:$A1000</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H11" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H101" type="list">
       <formula1>役職!$A$2:$A1000</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -801,8 +2036,8 @@
   </sheetPr>
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -811,48 +2046,68 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14"/>
+      <c r="A2" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14"/>
+      <c r="A3" s="13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15"/>
+      <c r="A5" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15"/>
+      <c r="A7" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15"/>
+      <c r="A9" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15"/>
+      <c r="A10" s="14" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15"/>
+      <c r="A11" s="14" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15"/>
+      <c r="A12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15"/>
+      <c r="A13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15"/>
+      <c r="A14" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -873,7 +2128,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -882,12 +2137,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16"/>
+      <c r="A2" s="15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>

</xml_diff>

<commit_message>
added trim  and probel cheklovi create by excell
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t xml:space="preserve">EmployeeID</t>
   </si>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">メールアドレス</t>
   </si>
   <si>
-    <t xml:space="preserve">DK01221</t>
+    <t xml:space="preserve">DK01251</t>
   </si>
   <si>
     <t xml:space="preserve">Ahmedov</t>
@@ -91,94 +91,58 @@
     <t xml:space="preserve">EMPLOYEE</t>
   </si>
   <si>
-    <t xml:space="preserve">1-department</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smm</t>
+    <t xml:space="preserve">広報部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tester</t>
   </si>
   <si>
     <t xml:space="preserve">11111111111uyf</t>
   </si>
   <si>
-    <t xml:space="preserve">nima11@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK01222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11111111112jhcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nima12@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK01223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nima13@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK01224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nima14@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nima15@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK01226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nima16@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK01227</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nima17gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK01240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nima18@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">７７７ｈ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nima19@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234567890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7-stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hghjs</t>
+    <t xml:space="preserve">nima41@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">管理本部123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">開発部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">人材開発育成事業部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-stage６６</t>
   </si>
   <si>
     <t xml:space="preserve">10-stage</t>
   </si>
   <si>
-    <t xml:space="preserve">656789787hhg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">656789787h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">656789787</t>
-  </si>
-  <si>
-    <t xml:space="preserve">098765432123456789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5-stage</t>
+    <t xml:space="preserve">Human resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital  Sale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">社長</t>
+  </si>
+  <si>
+    <t xml:space="preserve">部長</t>
+  </si>
+  <si>
+    <t xml:space="preserve">社員</t>
   </si>
 </sst>
 </file>
@@ -188,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -262,12 +226,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Noto Sans CJK JP"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -360,7 +318,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -405,11 +363,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -418,10 +376,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -677,7 +631,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -754,258 +708,92 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="10" t="n">
-        <v>11111111113</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="10" t="n">
-        <v>11111111115</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="10" t="n">
-        <v>11111111116</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="10" t="n">
-        <v>11111111117</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="10" t="n">
-        <v>11111111118</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="10" t="n">
-        <v>11111111119</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
@@ -2046,68 +1834,70 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>38</v>
+      <c r="A5" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>39</v>
+      <c r="A6" s="13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>40</v>
+      <c r="A7" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
-        <v>41</v>
+      <c r="A8" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
-        <v>42</v>
+      <c r="A9" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
-        <v>43</v>
+      <c r="A10" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
-        <v>44</v>
+      <c r="A11" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2128,7 +1918,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2137,32 +1927,44 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
fixed create by excel
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t xml:space="preserve">社員番号</t>
   </si>
@@ -54,13 +54,10 @@
     <t xml:space="preserve">メールアドレス</t>
   </si>
   <si>
-    <t xml:space="preserve">DK3342</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ahmedov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">角田さん</t>
+    <t xml:space="preserve">Ahmedov1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob1</t>
   </si>
   <si>
     <t xml:space="preserve">EMPLOYEE</t>
@@ -72,7 +69,103 @@
     <t xml:space="preserve">CEO</t>
   </si>
   <si>
-    <t xml:space="preserve">dfdsssd@gmail.com</t>
+    <t xml:space="preserve">suhrob1@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmedov2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kjhjgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suhrob2@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmedov3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suhrob3gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK0004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmedov4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suhrob4@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK0005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmedov5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１１１ｋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmedov6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suhrob6@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK0007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suhrob7@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmedov8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suhrob8@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK0009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmedov9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suhrob9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suhrob9@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">1-stage</t>
@@ -552,7 +645,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,117 +690,253 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
+      <c r="E4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="E5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="7"/>
+      <c r="J5" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
+      <c r="E6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="7"/>
+      <c r="J6" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="E7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
+      <c r="E8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="7"/>
+      <c r="J9" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="7"/>
+      <c r="J10" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
@@ -1754,12 +1983,12 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,12 +2058,12 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
changed edit by excell
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -63,10 +63,10 @@
     <t xml:space="preserve">EMPLOYEE</t>
   </si>
   <si>
-    <t xml:space="preserve">2-stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEO</t>
+    <t xml:space="preserve">ソフトウェア開発</t>
+  </si>
+  <si>
+    <t xml:space="preserve">プロダクトマネージャー </t>
   </si>
   <si>
     <t xml:space="preserve">suhrob1@gmail.com</t>
@@ -156,22 +156,22 @@
     <t xml:space="preserve">suhrob8@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">DK0009</t>
+    <t xml:space="preserve">DK0001</t>
   </si>
   <si>
     <t xml:space="preserve">Ahmedov9</t>
   </si>
   <si>
-    <t xml:space="preserve">Suhrob10</t>
+    <t xml:space="preserve">Suhrob9</t>
   </si>
   <si>
     <t xml:space="preserve">suhrob9@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">1-stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Engineer</t>
+    <t xml:space="preserve">製品管理 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DevOpsエンジニア </t>
   </si>
 </sst>
 </file>
@@ -332,7 +332,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -374,6 +374,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,7 +649,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -766,7 +770,7 @@
         <v>14</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -785,7 +789,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>13</v>
@@ -925,7 +929,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
@@ -1968,7 +1972,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1977,52 +1981,52 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13"/>
+      <c r="A6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
+      <c r="A7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13"/>
+      <c r="A8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
+      <c r="A11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
+      <c r="A12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
+      <c r="A14" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2043,7 +2047,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2052,18 +2056,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>49</v>
+      <c r="A2" s="15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>